<commit_message>
update: modified design document
</commit_message>
<xml_diff>
--- a/docs/DWH.Design.Template.xlsx
+++ b/docs/DWH.Design.Template.xlsx
@@ -10,7 +10,7 @@
     <sheet r:id="rId1" sheetId="1" name="ReadMe"/>
     <sheet r:id="rId2" sheetId="2" name="1.Business"/>
     <sheet r:id="rId3" sheetId="3" name="2.Tables"/>
-    <sheet r:id="rId4" sheetId="4" name="3.Cleaning&amp;amp;amp;amp;amp;amp;amp;amp;EDA"/>
+    <sheet r:id="rId4" sheetId="4" name="3.Cleaning&amp;amp;amp;amp;amp;amp;amp;amp;amp;EDA"/>
     <sheet r:id="rId5" sheetId="5" name="4.Dim.Tables"/>
     <sheet r:id="rId6" sheetId="6" name="5.Fact.Table"/>
     <sheet r:id="rId7" sheetId="7" name="6.Star Schema"/>
@@ -181,37 +181,41 @@
   </si>
   <si>
     <t>TrafficFlow
-TrafficFlow
+Accidents
 CongestionLevels
 Vehicles
-RoadConditions
 WeatherData
-TrafficLights
 SpeedViolations
 RoadClosures</t>
   </si>
   <si>
-    <t>1. Average Daily Traffic (ADT) by location
-2. Peak Hour Congestion Index
-3. Accident Rate per 100,000 vehicles
-4. Weather Impact on Traffic Flow
-5. Infrastructure Performance Metrics</t>
+    <t>Average Vehicle Count
+Incident Severity Index
+Peak Traffic Hour
+Congestion Level Score Trend
+Vehicles Involved per Incident
+Average Speed</t>
   </si>
   <si>
     <t>Potential Analytical Requirements of the Business</t>
   </si>
   <si>
-    <t xml:space="preserve">
-"What is the average vehicle speed by hour of day for each major intersection during peak hours?"
-"How does weather condition impact travel time across different districts?"
-"Which intersections experience the highest congestion during sporting events within a 2-mile radius?"
-"What is the monthly trend of traffic volume by vehicle type for each major corridor?"
-"How do holiday periods affect congestion patterns compared to regular weekdays?"
-"What is the correlation between precipitation levels and average travel time?"
-7. "Which intersections show the highest variance in throughput during construction periods?"
-"What is the impact of signal timing changes on queue lengths during peak hours?"
-"How does the congestion index vary by day of week and weather condition?"
-10. "What is the average delay time by vehicle type during different seasons?"</t>
+    <t>Peak Hour Analysis
+    Identify high traffic periods for congestion management and resource allocation.
+Event Type &amp; Severity Distribution
+    Understand the most frequent traffic events and their severity to prioritize interventions.
+Accident Risk Profiling
+    Determine high-risk time windows (day/time) to optimize road safety campaigns.
+Environmental Impact Assessment
+    Analyze how weather/road conditions impact traffic flow and accident rates.
+Vehicle-Type-Based Violations
+    Detect which vehicle types are most prone to speed violations to guide enforcement.
+Weekday vs. Weekend Traffic Behavior
+    Compare traffic dynamics on weekdays vs. weekends for better scheduling of maintenance and public transit.
+Seasonal Trend Analysis
+    Measure seasonal impact on traffic volumes for long-term planning.
+Traffic Volume Time-Series Trends
+    Monitor growth, decline, or anomalies in traffic volume over time.</t>
   </si>
   <si>
     <t>Specify the Grain (What will one row of the fact table represent?)</t>
@@ -2161,7 +2165,7 @@
       <c r="E12" s="88"/>
       <c r="F12" s="89"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="94" t="s">
         <v>52</v>
       </c>
@@ -2171,7 +2175,7 @@
       <c r="E13" s="94"/>
       <c r="F13" s="94"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="49">
       <c r="A14" s="82" t="s">
         <v>53</v>
       </c>
@@ -2181,7 +2185,7 @@
       <c r="E14" s="83"/>
       <c r="F14" s="84"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="49">
       <c r="A15" s="85"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -2189,7 +2193,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="86"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="82.2">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="49">
       <c r="A16" s="87"/>
       <c r="B16" s="88"/>
       <c r="C16" s="88"/>

</xml_diff>